<commit_message>
v1.2.20 from the developer
Commit includes fixes from the developer for repeated days.
</commit_message>
<xml_diff>
--- a/extras/sample-form/google calendar event sample [browser].xlsx
+++ b/extras/sample-form/google calendar event sample [browser].xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38081" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42312" uniqueCount="510">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3059,6 +3059,15 @@
   </si>
   <si>
     <t>custom-create-google-event(title=${event_title},description=${event_description},eventLocation=${event_location},eventTimezone=${event_timezone},repeatFrequency=${repeat_frequency},repeatWeekDays=${repeat_week_days},repeatEnd=${repeat_end},startDate=${start_date},endDate=${end_date})</t>
+  </si>
+  <si>
+    <t>Guests (a commas-separated list of valid email addresses)</t>
+  </si>
+  <si>
+    <t>custom-create-google-event(title=${event_title},description=${event_description},eventLocation=${event_location},guests=${guests},eventTimezone=${event_timezone},eventRepeatFrequency=${repeat_frequency},eventRepeatDays=${repeat_week_days},repeatEnd=${repeat_end},startDate=${start_date},endDate=${end_date})</t>
+  </si>
+  <si>
+    <t>Week days (Sun Mon Tue Wed Thu Fri Sat, Specified in a space-separated list)</t>
   </si>
 </sst>
 </file>
@@ -6886,7 +6895,7 @@
         <v>380</v>
       </c>
       <c r="K13" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="N13" t="s">
         <v>380</v>
@@ -6943,10 +6952,10 @@
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C16" t="s">
-        <v>471</v>
+        <v>507</v>
       </c>
       <c r="E16" t="s">
         <v>380</v>
@@ -6963,10 +6972,10 @@
         <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C17" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="E17" t="s">
         <v>380</v>
@@ -6983,10 +6992,10 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="C18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F18" t="s">
         <v>380</v>
@@ -7003,10 +7012,10 @@
         <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>483</v>
+        <v>496</v>
       </c>
       <c r="C19" t="s">
-        <v>482</v>
+        <v>500</v>
       </c>
       <c r="F19" t="s">
         <v>380</v>
@@ -7023,36 +7032,36 @@
         <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="C20" t="s">
-        <v>459</v>
+        <v>509</v>
       </c>
       <c r="F20" t="s">
-        <v>506</v>
+        <v>380</v>
       </c>
       <c r="K20" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>380</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>380</v>
+        <v>488</v>
       </c>
       <c r="C21" t="s">
-        <v>380</v>
+        <v>459</v>
       </c>
       <c r="F21" t="s">
-        <v>380</v>
+        <v>508</v>
       </c>
       <c r="I21" t="s">
         <v>380</v>
       </c>
       <c r="K21" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
     </row>
     <row r="22">
@@ -7388,7 +7397,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f>TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006301339</v>
+        <v>2007031542</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>380</v>

</xml_diff>